<commit_message>
Added a bunch of string parsing and opcode functions to assembler
</commit_message>
<xml_diff>
--- a/Documentation/CSPARC_ISA.xlsx
+++ b/Documentation/CSPARC_ISA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="I-Formats" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="263">
   <si>
     <t>Operand-Register Type</t>
   </si>
@@ -796,6 +796,18 @@
   </si>
   <si>
     <t>S-type 1 signifies arithmetic, RSA</t>
+  </si>
+  <si>
+    <t>111 110</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>111 111</t>
+  </si>
+  <si>
+    <t>No-op</t>
   </si>
 </sst>
 </file>
@@ -846,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -912,6 +924,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1328,10 +1349,10 @@
       <c r="E6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="10" t="s">
         <v>56</v>
       </c>
@@ -1346,10 +1367,10 @@
       <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="10" t="s">
         <v>57</v>
       </c>
@@ -1367,10 +1388,10 @@
       <c r="E8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="12">
         <v>1</v>
       </c>
@@ -1393,10 +1414,10 @@
       <c r="E10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="10" t="s">
         <v>62</v>
       </c>
@@ -1411,10 +1432,10 @@
       <c r="E11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="10" t="s">
         <v>57</v>
       </c>
@@ -1432,10 +1453,10 @@
       <c r="E12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="33"/>
+      <c r="F12" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="36"/>
       <c r="H12" s="14" t="s">
         <v>22</v>
       </c>
@@ -1453,10 +1474,10 @@
       <c r="F14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="2:9">
       <c r="C15" s="10" t="s">
@@ -1471,10 +1492,10 @@
       <c r="F15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" t="s">
@@ -1492,10 +1513,10 @@
       <c r="F16" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="33"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="17" t="s">
         <v>68</v>
       </c>
@@ -1510,11 +1531,11 @@
       <c r="E17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="18" t="s">
         <v>69</v>
       </c>
@@ -1537,11 +1558,11 @@
       <c r="E19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="2:9">
       <c r="C20" s="10" t="s">
@@ -1553,11 +1574,11 @@
       <c r="E20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" t="s">
@@ -1572,11 +1593,11 @@
       <c r="E21" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
       <c r="I21" t="s">
         <v>72</v>
       </c>
@@ -1591,11 +1612,11 @@
       <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
       <c r="I22" t="s">
         <v>73</v>
       </c>
@@ -1613,10 +1634,10 @@
       <c r="F24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="29"/>
+      <c r="G24" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="32"/>
     </row>
     <row r="25" spans="2:9">
       <c r="C25" s="10" t="s">
@@ -1631,10 +1652,10 @@
       <c r="F25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H25" s="30"/>
+      <c r="H25" s="33"/>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" t="s">
@@ -1652,10 +1673,10 @@
       <c r="F26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="31"/>
+      <c r="G26" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="34"/>
     </row>
     <row r="28" spans="2:9">
       <c r="B28" t="s">
@@ -1691,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1710,15 +1731,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="4"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2039,15 +2060,15 @@
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:13">
@@ -2061,10 +2082,10 @@
       <c r="E14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="10" t="s">
         <v>56</v>
       </c>
@@ -2081,10 +2102,10 @@
       <c r="E15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="10" t="s">
         <v>57</v>
       </c>
@@ -2112,10 +2133,10 @@
       <c r="E16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="34"/>
+      <c r="G16" s="37"/>
       <c r="H16" s="12">
         <v>1</v>
       </c>
@@ -2140,10 +2161,10 @@
       <c r="E17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="34"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="12">
         <v>1</v>
       </c>
@@ -2170,10 +2191,10 @@
       <c r="E18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="34"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="15">
         <v>1</v>
       </c>
@@ -2200,10 +2221,10 @@
       <c r="E19" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="34"/>
+      <c r="G19" s="37"/>
       <c r="H19" s="15">
         <v>1</v>
       </c>
@@ -2230,10 +2251,10 @@
       <c r="E20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="34"/>
+      <c r="G20" s="37"/>
       <c r="H20" s="12">
         <v>1</v>
       </c>
@@ -2258,10 +2279,10 @@
       <c r="E21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="34"/>
+      <c r="G21" s="37"/>
       <c r="H21" s="12">
         <v>1</v>
       </c>
@@ -2286,10 +2307,10 @@
       <c r="E22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="34"/>
+      <c r="G22" s="37"/>
       <c r="H22" s="12">
         <v>1</v>
       </c>
@@ -2302,15 +2323,15 @@
       </c>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="2:13">
@@ -2323,10 +2344,10 @@
       <c r="E25" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="30"/>
+      <c r="G25" s="33"/>
       <c r="H25" s="10" t="s">
         <v>62</v>
       </c>
@@ -2343,10 +2364,10 @@
       <c r="E26" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="33"/>
       <c r="H26" s="10" t="s">
         <v>57</v>
       </c>
@@ -2374,10 +2395,10 @@
       <c r="E27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="33"/>
+      <c r="G27" s="36"/>
       <c r="H27" s="12" t="s">
         <v>62</v>
       </c>
@@ -2405,10 +2426,10 @@
       <c r="E28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="33"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="4" t="s">
         <v>62</v>
       </c>
@@ -2427,8 +2448,8 @@
       <c r="C29" s="4"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="33"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
@@ -2436,8 +2457,8 @@
       <c r="C30" s="4"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="33"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
@@ -2473,7 +2494,7 @@
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2489,15 +2510,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="4"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2517,10 +2538,10 @@
       <c r="F3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="29"/>
+      <c r="G3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="32"/>
       <c r="I3" s="10"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2540,10 +2561,10 @@
       <c r="F4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="30"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="10"/>
       <c r="J4" s="3" t="s">
         <v>107</v>
@@ -2571,10 +2592,10 @@
       <c r="F5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="31"/>
+      <c r="G5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="34"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
         <v>110</v>
@@ -2600,10 +2621,10 @@
       <c r="F6" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="31"/>
+      <c r="G6" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="34"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12" t="s">
         <v>111</v>
@@ -2628,10 +2649,10 @@
       <c r="F7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="31"/>
+      <c r="G7" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="34"/>
       <c r="I7" s="13"/>
       <c r="J7" s="12" t="s">
         <v>112</v>
@@ -2659,10 +2680,10 @@
       <c r="F8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="31"/>
+      <c r="G8" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="34"/>
       <c r="I8" s="13"/>
       <c r="J8" s="12" t="s">
         <v>113</v>
@@ -2690,10 +2711,10 @@
       <c r="F9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="31"/>
+      <c r="G9" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="34"/>
       <c r="I9" s="13"/>
       <c r="J9" s="25" t="s">
         <v>249</v>
@@ -2718,10 +2739,10 @@
       <c r="F10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="31"/>
+      <c r="G10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="34"/>
       <c r="I10" s="13"/>
       <c r="J10" s="12" t="s">
         <v>120</v>
@@ -2835,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2850,15 +2871,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="4"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2872,12 +2893,12 @@
       <c r="D3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="10"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2891,12 +2912,12 @@
       <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="10"/>
       <c r="J4" s="3" t="s">
         <v>107</v>
@@ -2916,12 +2937,12 @@
       <c r="D5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
         <v>125</v>
@@ -2937,8 +2958,8 @@
       <c r="D6" s="4"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="18" t="s">
@@ -2946,15 +2967,15 @@
       </c>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="4"/>
@@ -2972,10 +2993,10 @@
       <c r="F8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="H8" s="33"/>
     </row>
     <row r="9" spans="2:12">
       <c r="C9" s="10" t="s">
@@ -2990,10 +3011,10 @@
       <c r="F9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="33"/>
       <c r="J9" s="3" t="s">
         <v>107</v>
       </c>
@@ -3006,22 +3027,22 @@
       <c r="B10" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="28"/>
+      <c r="H10" s="31"/>
       <c r="J10" t="s">
         <v>132</v>
       </c>
@@ -3033,22 +3054,22 @@
       <c r="B11" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="30" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="28"/>
+      <c r="H11" s="31"/>
       <c r="J11" t="s">
         <v>137</v>
       </c>
@@ -3060,22 +3081,22 @@
       <c r="B12" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="30" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="28"/>
+      <c r="H12" s="31"/>
       <c r="J12" t="s">
         <v>136</v>
       </c>
@@ -3138,15 +3159,15 @@
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="4"/>
@@ -3158,12 +3179,12 @@
       <c r="D23" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="2:11">
@@ -3173,12 +3194,12 @@
       <c r="D24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
       <c r="I24" s="16"/>
       <c r="J24" s="3" t="s">
         <v>107</v>
@@ -3197,12 +3218,12 @@
       <c r="D25" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="19"/>
       <c r="J25" s="18" t="s">
         <v>158</v>
@@ -3221,12 +3242,12 @@
       <c r="D26" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
+      <c r="E26" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
       <c r="J26" s="18" t="s">
         <v>161</v>
       </c>
@@ -3244,12 +3265,12 @@
       <c r="D27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
       <c r="J27" s="18" t="s">
         <v>229</v>
       </c>
@@ -3267,12 +3288,12 @@
       <c r="D28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="E28" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="12"/>
       <c r="J28" s="17" t="s">
         <v>176</v>
@@ -3347,7 +3368,7 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3360,17 +3381,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="2:12">
       <c r="B2" s="2"/>
@@ -3383,11 +3404,11 @@
       <c r="E2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
@@ -3402,11 +3423,11 @@
       <c r="E3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
         <v>181</v>
@@ -3431,11 +3452,11 @@
       <c r="E4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
       <c r="I4" s="7"/>
       <c r="J4" t="s">
         <v>29</v>
@@ -3457,11 +3478,11 @@
       <c r="E5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="7"/>
       <c r="J5" t="s">
         <v>213</v>
@@ -3483,11 +3504,11 @@
       <c r="E6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="7"/>
       <c r="J6" s="18" t="s">
         <v>214</v>
@@ -3512,11 +3533,11 @@
       <c r="E7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
       <c r="J7" s="18" t="s">
         <v>215</v>
       </c>
@@ -3540,11 +3561,11 @@
       <c r="E8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="F8" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="7"/>
       <c r="J8" t="s">
         <v>216</v>
@@ -3569,11 +3590,11 @@
       <c r="E9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="F9" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="7"/>
       <c r="J9" t="s">
         <v>185</v>
@@ -3595,11 +3616,11 @@
       <c r="E10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="F10" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="7"/>
       <c r="J10" t="s">
         <v>187</v>
@@ -3612,9 +3633,9 @@
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:12">
@@ -3650,11 +3671,11 @@
       <c r="E16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
@@ -3669,11 +3690,11 @@
       <c r="E17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="4"/>
       <c r="J17" s="3" t="s">
         <v>181</v>
@@ -3698,11 +3719,11 @@
       <c r="E18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
       <c r="I18" s="7"/>
       <c r="J18" t="s">
         <v>40</v>
@@ -3724,11 +3745,11 @@
       <c r="E19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="7"/>
       <c r="J19" t="s">
         <v>211</v>
@@ -3750,11 +3771,11 @@
       <c r="E20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="7"/>
       <c r="J20" s="18" t="s">
         <v>212</v>
@@ -3779,11 +3800,11 @@
       <c r="E21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
       <c r="J21" s="18" t="s">
         <v>210</v>
       </c>
@@ -3807,11 +3828,11 @@
       <c r="E22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="F22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="7"/>
       <c r="J22" t="s">
         <v>217</v>
@@ -3836,11 +3857,11 @@
       <c r="E23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
+      <c r="F23" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
       <c r="I23" s="7"/>
       <c r="J23" t="s">
         <v>220</v>
@@ -3862,11 +3883,11 @@
       <c r="E24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
+      <c r="F24" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="7"/>
       <c r="J24" t="s">
         <v>221</v>
@@ -3919,7 +3940,7 @@
   <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3933,15 +3954,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="22"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3961,10 +3982,10 @@
       <c r="F2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="29"/>
+      <c r="G2" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="32"/>
       <c r="I2" s="23"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
@@ -3984,10 +4005,10 @@
       <c r="F3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="23"/>
       <c r="J3" s="3" t="s">
         <v>107</v>
@@ -4015,18 +4036,18 @@
       <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="31"/>
+      <c r="G4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="34"/>
       <c r="I4" s="24"/>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="6" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4034,8 +4055,8 @@
       <c r="B5" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>252</v>
+      <c r="C5" s="28" t="s">
+        <v>259</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>252</v>
@@ -4046,17 +4067,59 @@
       <c r="F5" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="24"/>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="6" t="s">
         <v>254</v>
       </c>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="34"/>
+      <c r="J6" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="5" t="s">
@@ -4123,7 +4186,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="G5:H5"/>

</xml_diff>

<commit_message>
Added more functions to assembler, now parsing the string and decoding the opcode into separate functions.
</commit_message>
<xml_diff>
--- a/Documentation/CSPARC_ISA.xlsx
+++ b/Documentation/CSPARC_ISA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="I-Formats" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="264">
   <si>
     <t>Operand-Register Type</t>
   </si>
@@ -808,6 +808,9 @@
   </si>
   <si>
     <t>No-op</t>
+  </si>
+  <si>
+    <t>100 110</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -943,22 +946,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1349,10 +1355,10 @@
       <c r="E6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="10" t="s">
         <v>56</v>
       </c>
@@ -1367,10 +1373,10 @@
       <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="33"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="10" t="s">
         <v>57</v>
       </c>
@@ -1388,10 +1394,10 @@
       <c r="E8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="12">
         <v>1</v>
       </c>
@@ -1414,10 +1420,10 @@
       <c r="E10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="33"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="10" t="s">
         <v>62</v>
       </c>
@@ -1432,10 +1438,10 @@
       <c r="E11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="33"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="10" t="s">
         <v>57</v>
       </c>
@@ -1453,10 +1459,10 @@
       <c r="E12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="36"/>
+      <c r="F12" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="33"/>
       <c r="H12" s="14" t="s">
         <v>22</v>
       </c>
@@ -1474,10 +1480,10 @@
       <c r="F14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="33"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="2:9">
       <c r="C15" s="10" t="s">
@@ -1492,10 +1498,10 @@
       <c r="F15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="33"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" t="s">
@@ -1513,10 +1519,10 @@
       <c r="F16" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="36"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="17" t="s">
         <v>68</v>
       </c>
@@ -1531,11 +1537,11 @@
       <c r="E17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="18" t="s">
         <v>69</v>
       </c>
@@ -1558,11 +1564,11 @@
       <c r="E19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="2:9">
       <c r="C20" s="10" t="s">
@@ -1574,11 +1580,11 @@
       <c r="E20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" t="s">
@@ -1593,11 +1599,11 @@
       <c r="E21" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
       <c r="I21" t="s">
         <v>72</v>
       </c>
@@ -1612,11 +1618,11 @@
       <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
       <c r="I22" t="s">
         <v>73</v>
       </c>
@@ -1634,10 +1640,10 @@
       <c r="F24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="32"/>
+      <c r="G24" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="2:9">
       <c r="C25" s="10" t="s">
@@ -1652,10 +1658,10 @@
       <c r="F25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H25" s="33"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" t="s">
@@ -1673,10 +1679,10 @@
       <c r="F26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="34"/>
+      <c r="G26" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="38"/>
     </row>
     <row r="28" spans="2:9">
       <c r="B28" t="s">
@@ -1685,6 +1691,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
@@ -1694,14 +1708,6 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1731,15 +1737,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
       <c r="I1" s="4"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2060,15 +2066,15 @@
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:13">
@@ -2082,10 +2088,10 @@
       <c r="E14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="33"/>
+      <c r="G14" s="34"/>
       <c r="H14" s="10" t="s">
         <v>56</v>
       </c>
@@ -2102,10 +2108,10 @@
       <c r="E15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="33"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="10" t="s">
         <v>57</v>
       </c>
@@ -2133,10 +2139,10 @@
       <c r="E16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="12">
         <v>1</v>
       </c>
@@ -2161,10 +2167,10 @@
       <c r="E17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="37"/>
+      <c r="G17" s="35"/>
       <c r="H17" s="12">
         <v>1</v>
       </c>
@@ -2191,10 +2197,10 @@
       <c r="E18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="37"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="15">
         <v>1</v>
       </c>
@@ -2221,10 +2227,10 @@
       <c r="E19" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="37"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="15">
         <v>1</v>
       </c>
@@ -2251,10 +2257,10 @@
       <c r="E20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="37"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="12">
         <v>1</v>
       </c>
@@ -2279,10 +2285,10 @@
       <c r="E21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="37"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="12">
         <v>1</v>
       </c>
@@ -2307,10 +2313,10 @@
       <c r="E22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="F22" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="37"/>
+      <c r="G22" s="35"/>
       <c r="H22" s="12">
         <v>1</v>
       </c>
@@ -2323,15 +2329,15 @@
       </c>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="2:13">
@@ -2344,10 +2350,10 @@
       <c r="E25" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="10" t="s">
         <v>62</v>
       </c>
@@ -2364,10 +2370,10 @@
       <c r="E26" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="33"/>
+      <c r="G26" s="34"/>
       <c r="H26" s="10" t="s">
         <v>57</v>
       </c>
@@ -2395,10 +2401,10 @@
       <c r="E27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="36"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="12" t="s">
         <v>62</v>
       </c>
@@ -2426,10 +2432,10 @@
       <c r="E28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="36"/>
+      <c r="G28" s="33"/>
       <c r="H28" s="4" t="s">
         <v>62</v>
       </c>
@@ -2448,8 +2454,8 @@
       <c r="C29" s="4"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="33"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
@@ -2457,18 +2463,18 @@
       <c r="C30" s="4"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="33"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F26:G26"/>
@@ -2477,11 +2483,11 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2510,15 +2516,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="4"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2538,10 +2544,10 @@
       <c r="F3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="32"/>
+      <c r="G3" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="37"/>
       <c r="I3" s="10"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2561,10 +2567,10 @@
       <c r="F4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="10"/>
       <c r="J4" s="3" t="s">
         <v>107</v>
@@ -2592,10 +2598,10 @@
       <c r="F5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="34"/>
+      <c r="G5" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="38"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
         <v>110</v>
@@ -2621,10 +2627,10 @@
       <c r="F6" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="34"/>
+      <c r="G6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="38"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12" t="s">
         <v>111</v>
@@ -2649,10 +2655,10 @@
       <c r="F7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="34"/>
+      <c r="G7" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="38"/>
       <c r="I7" s="13"/>
       <c r="J7" s="12" t="s">
         <v>112</v>
@@ -2680,10 +2686,10 @@
       <c r="F8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="34"/>
+      <c r="G8" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="38"/>
       <c r="I8" s="13"/>
       <c r="J8" s="12" t="s">
         <v>113</v>
@@ -2711,10 +2717,10 @@
       <c r="F9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="34"/>
+      <c r="G9" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="38"/>
       <c r="I9" s="13"/>
       <c r="J9" s="25" t="s">
         <v>249</v>
@@ -2739,10 +2745,10 @@
       <c r="F10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="34"/>
+      <c r="G10" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="38"/>
       <c r="I10" s="13"/>
       <c r="J10" s="12" t="s">
         <v>120</v>
@@ -2856,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2871,15 +2877,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="4"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2893,12 +2899,12 @@
       <c r="D3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="10"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2912,12 +2918,12 @@
       <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="10"/>
       <c r="J4" s="3" t="s">
         <v>107</v>
@@ -2937,12 +2943,12 @@
       <c r="D5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
         <v>125</v>
@@ -2958,8 +2964,8 @@
       <c r="D6" s="4"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="18" t="s">
@@ -2967,15 +2973,15 @@
       </c>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="4"/>
@@ -2993,10 +2999,10 @@
       <c r="F8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="33"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="2:12">
       <c r="C9" s="10" t="s">
@@ -3011,10 +3017,10 @@
       <c r="F9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="33"/>
+      <c r="H9" s="34"/>
       <c r="J9" s="3" t="s">
         <v>107</v>
       </c>
@@ -3039,10 +3045,10 @@
       <c r="F10" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="31"/>
+      <c r="H10" s="36"/>
       <c r="J10" t="s">
         <v>132</v>
       </c>
@@ -3066,10 +3072,10 @@
       <c r="F11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="31"/>
+      <c r="H11" s="36"/>
       <c r="J11" t="s">
         <v>137</v>
       </c>
@@ -3093,10 +3099,10 @@
       <c r="F12" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="31"/>
+      <c r="H12" s="36"/>
       <c r="J12" t="s">
         <v>136</v>
       </c>
@@ -3159,15 +3165,15 @@
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="4"/>
@@ -3179,12 +3185,12 @@
       <c r="D23" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="2:11">
@@ -3194,12 +3200,12 @@
       <c r="D24" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="16"/>
       <c r="J24" s="3" t="s">
         <v>107</v>
@@ -3218,12 +3224,12 @@
       <c r="D25" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="19"/>
       <c r="J25" s="18" t="s">
         <v>158</v>
@@ -3242,12 +3248,12 @@
       <c r="D26" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
+      <c r="E26" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
       <c r="J26" s="18" t="s">
         <v>161</v>
       </c>
@@ -3265,12 +3271,12 @@
       <c r="D27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
       <c r="J27" s="18" t="s">
         <v>229</v>
       </c>
@@ -3288,12 +3294,12 @@
       <c r="D28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
+      <c r="E28" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
       <c r="I28" s="12"/>
       <c r="J28" s="17" t="s">
         <v>176</v>
@@ -3340,6 +3346,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="E4:H4"/>
@@ -3347,17 +3364,6 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3368,7 +3374,7 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3381,17 +3387,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="2:12">
       <c r="B2" s="2"/>
@@ -3404,11 +3410,11 @@
       <c r="E2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
@@ -3423,11 +3429,11 @@
       <c r="E3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
         <v>181</v>
@@ -3443,8 +3449,8 @@
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>162</v>
+      <c r="C4" s="31" t="s">
+        <v>163</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
@@ -3452,11 +3458,11 @@
       <c r="E4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="7"/>
       <c r="J4" t="s">
         <v>29</v>
@@ -3469,8 +3475,8 @@
       <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>163</v>
+      <c r="C5" s="31" t="s">
+        <v>164</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>20</v>
@@ -3478,11 +3484,11 @@
       <c r="E5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="7"/>
       <c r="J5" t="s">
         <v>213</v>
@@ -3495,8 +3501,8 @@
       <c r="B6" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>164</v>
+      <c r="C6" s="31" t="s">
+        <v>165</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>20</v>
@@ -3504,11 +3510,11 @@
       <c r="E6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="7"/>
       <c r="J6" s="18" t="s">
         <v>214</v>
@@ -3524,8 +3530,8 @@
       <c r="B7" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>165</v>
+      <c r="C7" s="31" t="s">
+        <v>166</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>20</v>
@@ -3533,11 +3539,11 @@
       <c r="E7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="J7" s="18" t="s">
         <v>215</v>
       </c>
@@ -3552,8 +3558,8 @@
       <c r="B8" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>166</v>
+      <c r="C8" s="31" t="s">
+        <v>167</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>23</v>
@@ -3561,11 +3567,11 @@
       <c r="E8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="7"/>
       <c r="J8" t="s">
         <v>216</v>
@@ -3581,8 +3587,8 @@
       <c r="B9" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>167</v>
+      <c r="C9" s="31" t="s">
+        <v>168</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
@@ -3590,11 +3596,11 @@
       <c r="E9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
       <c r="I9" s="7"/>
       <c r="J9" t="s">
         <v>185</v>
@@ -3607,8 +3613,8 @@
       <c r="B10" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>168</v>
+      <c r="C10" s="31" t="s">
+        <v>169</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>23</v>
@@ -3616,11 +3622,11 @@
       <c r="E10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="F10" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="7"/>
       <c r="J10" t="s">
         <v>187</v>
@@ -3633,9 +3639,9 @@
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:12">
@@ -3671,11 +3677,11 @@
       <c r="E16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
@@ -3690,11 +3696,11 @@
       <c r="E17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="4"/>
       <c r="J17" s="3" t="s">
         <v>181</v>
@@ -3710,8 +3716,8 @@
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>169</v>
+      <c r="C18" s="31" t="s">
+        <v>170</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
@@ -3719,11 +3725,11 @@
       <c r="E18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="7"/>
       <c r="J18" t="s">
         <v>40</v>
@@ -3736,8 +3742,8 @@
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>170</v>
+      <c r="C19" s="31" t="s">
+        <v>200</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>20</v>
@@ -3745,11 +3751,11 @@
       <c r="E19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
       <c r="I19" s="7"/>
       <c r="J19" t="s">
         <v>211</v>
@@ -3762,8 +3768,8 @@
       <c r="B20" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>200</v>
+      <c r="C20" s="31" t="s">
+        <v>201</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
@@ -3771,11 +3777,11 @@
       <c r="E20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
       <c r="I20" s="7"/>
       <c r="J20" s="18" t="s">
         <v>212</v>
@@ -3791,8 +3797,8 @@
       <c r="B21" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>201</v>
+      <c r="C21" s="31" t="s">
+        <v>202</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>20</v>
@@ -3800,11 +3806,11 @@
       <c r="E21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
       <c r="J21" s="18" t="s">
         <v>210</v>
       </c>
@@ -3819,8 +3825,8 @@
       <c r="B22" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>202</v>
+      <c r="C22" s="31" t="s">
+        <v>203</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>23</v>
@@ -3828,11 +3834,11 @@
       <c r="E22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="F22" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="7"/>
       <c r="J22" t="s">
         <v>217</v>
@@ -3848,8 +3854,8 @@
       <c r="B23" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>203</v>
+      <c r="C23" s="31" t="s">
+        <v>204</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>20</v>
@@ -3857,11 +3863,11 @@
       <c r="E23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
+      <c r="F23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
       <c r="I23" s="7"/>
       <c r="J23" t="s">
         <v>220</v>
@@ -3874,8 +3880,8 @@
       <c r="B24" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>204</v>
+      <c r="C24" s="31" t="s">
+        <v>247</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>23</v>
@@ -3883,11 +3889,11 @@
       <c r="E24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="F24" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="7"/>
       <c r="J24" t="s">
         <v>221</v>
@@ -3910,16 +3916,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
@@ -3930,6 +3926,16 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3939,8 +3945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3954,15 +3960,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
       <c r="I1" s="22"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -3982,10 +3988,10 @@
       <c r="F2" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="32"/>
+      <c r="G2" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="37"/>
       <c r="I2" s="23"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
@@ -4005,10 +4011,10 @@
       <c r="F3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="33"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="23"/>
       <c r="J3" s="3" t="s">
         <v>107</v>
@@ -4024,8 +4030,8 @@
       <c r="B4" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>247</v>
+      <c r="C4" s="31" t="s">
+        <v>263</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>20</v>
@@ -4036,10 +4042,10 @@
       <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="34"/>
+      <c r="G4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="38"/>
       <c r="I4" s="24"/>
       <c r="J4" s="19" t="s">
         <v>231</v>
@@ -4055,7 +4061,7 @@
       <c r="B5" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="31" t="s">
         <v>259</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -4067,10 +4073,10 @@
       <c r="F5" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="H5" s="34"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="24"/>
       <c r="J5" s="19" t="s">
         <v>253</v>
@@ -4096,10 +4102,10 @@
       <c r="F6" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="H6" s="34"/>
+      <c r="H6" s="38"/>
       <c r="J6" s="6" t="s">
         <v>262</v>
       </c>

</xml_diff>